<commit_message>
Update Security Program Tracking Template.xlsx
</commit_message>
<xml_diff>
--- a/Security Program Tracking Template.xlsx
+++ b/Security Program Tracking Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omnissa-my.sharepoint.com/personal/msnyder_omnissa_com/Documents/Documents/GitHub/security_maturity_tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omnissa-my.sharepoint.com/personal/msnyder_omnissa_com/Documents/Documents/GitHub/security_maturity_tracker/Security-Maturity-Tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{2630C45D-FD86-FD44-B917-8461A07E36E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B75118F-1D38-0046-AA2D-02FFF35CDD2D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{482FF75D-DA18-3646-9B45-A2B35A9B0AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="2560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B26B179B-1624-BB4A-B266-612C886FC91F}"/>
+    <workbookView xWindow="1060" yWindow="2560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B26B179B-1624-BB4A-B266-612C886FC91F}"/>
   </bookViews>
   <sheets>
     <sheet name="Program Overview" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="259">
   <si>
     <t>Metric Name</t>
   </si>
@@ -712,9 +712,6 @@
     <t>Data Access Monitoring</t>
   </si>
   <si>
-    <t>ERP System Logs (SAP)</t>
-  </si>
-  <si>
     <t>Financial Monitoring, Compliance</t>
   </si>
   <si>
@@ -743,6 +740,105 @@
   </si>
   <si>
     <t>Compliance Requirements</t>
+  </si>
+  <si>
+    <t>Enterprise Resource Planning (ERP) System Logs (SAP)</t>
+  </si>
+  <si>
+    <t>Capability</t>
+  </si>
+  <si>
+    <t>Detection Capabilities</t>
+  </si>
+  <si>
+    <t>Ability to detect various threats, such as malware, anomalies, and insider threats using the SIEM.</t>
+  </si>
+  <si>
+    <t>Partially Available</t>
+  </si>
+  <si>
+    <t>SIEM Team</t>
+  </si>
+  <si>
+    <t>Improve detection rules for insider threats</t>
+  </si>
+  <si>
+    <t>Threat Hunting</t>
+  </si>
+  <si>
+    <t>Ability to proactively search for indicators of compromise (IOCs) and unknown threats.</t>
+  </si>
+  <si>
+    <t>Threat Intel Team</t>
+  </si>
+  <si>
+    <t>Increase frequency of threat hunts</t>
+  </si>
+  <si>
+    <t>Threat Detection, Incident Response</t>
+  </si>
+  <si>
+    <t>Custom Dashboards</t>
+  </si>
+  <si>
+    <t>Customizable dashboards to monitor specific activities or use cases.</t>
+  </si>
+  <si>
+    <t>Develop more user-specific dashboards</t>
+  </si>
+  <si>
+    <t>Visibility, Reporting, Compliance</t>
+  </si>
+  <si>
+    <t>Alert Creation</t>
+  </si>
+  <si>
+    <t>Ability to create and manage alerts for suspicious activities detected in logs.</t>
+  </si>
+  <si>
+    <t>SOC Team</t>
+  </si>
+  <si>
+    <t>Refine alert thresholds to reduce false positives</t>
+  </si>
+  <si>
+    <t>Admin Functions</t>
+  </si>
+  <si>
+    <t>Administrative tasks such as user management, log retention, and configuration changes.</t>
+  </si>
+  <si>
+    <t>Streamline user role assignment</t>
+  </si>
+  <si>
+    <t>System Management, Compliance</t>
+  </si>
+  <si>
+    <t>Upkeep</t>
+  </si>
+  <si>
+    <t>Regular maintenance, software updates, and system health checks for the SIEM.</t>
+  </si>
+  <si>
+    <t>SIEM Maintenance Team</t>
+  </si>
+  <si>
+    <t>Automate routine maintenance tasks</t>
+  </si>
+  <si>
+    <t>System Stability, Compliance</t>
+  </si>
+  <si>
+    <t>Threat Intel Feed Search</t>
+  </si>
+  <si>
+    <t>Capability to search for and correlate threat intelligence feeds with internal activity to identify threats.</t>
+  </si>
+  <si>
+    <t>Integrate additional threat feeds</t>
+  </si>
+  <si>
+    <t>Threat Detection, Threat Intelligence</t>
   </si>
 </sst>
 </file>
@@ -1575,13 +1671,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7390EF0B-64A1-0F43-933C-C752CDDB3F1B}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
@@ -1613,7 +1709,7 @@
         <v>94</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>95</v>
@@ -2755,7 +2851,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>170</v>
@@ -2777,7 +2873,7 @@
         <v>109</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>111</v>
@@ -2786,7 +2882,7 @@
         <v>112</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>114</v>
@@ -2803,7 +2899,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>170</v>
@@ -2825,7 +2921,7 @@
         <v>120</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>111</v>
@@ -2834,7 +2930,7 @@
         <v>112</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>114</v>
@@ -2851,7 +2947,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>118</v>
@@ -2873,7 +2969,7 @@
         <v>171</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>111</v>
@@ -2899,7 +2995,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>118</v>
@@ -2921,7 +3017,7 @@
         <v>120</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>111</v>
@@ -2952,12 +3048,208 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350E66AA-AE30-8D42-A85F-0F2DA245F843}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>